<commit_message>
work on legit everything else except the creation of servers
</commit_message>
<xml_diff>
--- a/P10/full_credit/JADE_Scrum_Sprint_4.xlsx
+++ b/P10/full_credit/JADE_Scrum_Sprint_4.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="196">
   <si>
     <t xml:space="preserve">Product Name:</t>
   </si>
@@ -269,6 +269,9 @@
     <t xml:space="preserve">CS</t>
   </si>
   <si>
+    <t xml:space="preserve">Finished in Sprint 5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Create a new named server</t>
   </si>
   <si>
@@ -276,6 +279,9 @@
   </si>
   <si>
     <t xml:space="preserve">CO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Work</t>
   </si>
   <si>
     <t xml:space="preserve">Create an order of multiple products</t>
@@ -1054,343 +1060,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Product Backlog Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.0821832261287704"/>
-          <c:y val="0.161875945537065"/>
-          <c:w val="0.884343970523949"/>
-          <c:h val="0.63565305093293"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:scatterChart>
-        <c:scatterStyle val="line"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Product Backlog'!$A$12:$A$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Product Backlog'!$B$12:$B$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:axId val="40440027"/>
-        <c:axId val="65796667"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="40440027"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="6"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Sprints</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="65796667"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="65796667"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Features Remaining at end of Sprint</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="40440027"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="span"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1518,11 +1188,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="82904133"/>
-        <c:axId val="94090473"/>
+        <c:axId val="45939029"/>
+        <c:axId val="51949459"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82904133"/>
+        <c:axId val="45939029"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1587,7 +1257,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94090473"/>
+        <c:crossAx val="51949459"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1595,7 +1265,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94090473"/>
+        <c:axId val="51949459"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1669,7 +1339,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82904133"/>
+        <c:crossAx val="45939029"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1689,14 +1359,14 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1824,11 +1494,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="74736521"/>
-        <c:axId val="30095726"/>
+        <c:axId val="73376012"/>
+        <c:axId val="91645951"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="74736521"/>
+        <c:axId val="73376012"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1893,7 +1563,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30095726"/>
+        <c:crossAx val="91645951"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1901,7 +1571,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30095726"/>
+        <c:axId val="91645951"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1975,7 +1645,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74736521"/>
+        <c:crossAx val="73376012"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1995,14 +1665,14 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2130,11 +1800,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="78190013"/>
-        <c:axId val="41523317"/>
+        <c:axId val="61886598"/>
+        <c:axId val="66937973"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="78190013"/>
+        <c:axId val="61886598"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2199,7 +1869,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41523317"/>
+        <c:crossAx val="66937973"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2207,7 +1877,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41523317"/>
+        <c:axId val="66937973"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2281,7 +1951,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78190013"/>
+        <c:crossAx val="61886598"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2301,14 +1971,14 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2436,11 +2106,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="25477726"/>
-        <c:axId val="1623010"/>
+        <c:axId val="12311503"/>
+        <c:axId val="49710203"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="25477726"/>
+        <c:axId val="12311503"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2505,7 +2175,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1623010"/>
+        <c:crossAx val="49710203"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2513,7 +2183,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1623010"/>
+        <c:axId val="49710203"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2587,7 +2257,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25477726"/>
+        <c:crossAx val="12311503"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2607,14 +2277,14 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2727,7 +2397,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2742,11 +2412,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="80031259"/>
-        <c:axId val="48038994"/>
+        <c:axId val="6653526"/>
+        <c:axId val="10969325"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80031259"/>
+        <c:axId val="6653526"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2811,7 +2481,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48038994"/>
+        <c:crossAx val="10969325"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2819,7 +2489,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48038994"/>
+        <c:axId val="10969325"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2893,7 +2563,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80031259"/>
+        <c:crossAx val="6653526"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2913,14 +2583,14 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3048,11 +2718,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="83870235"/>
-        <c:axId val="86159457"/>
+        <c:axId val="52901568"/>
+        <c:axId val="2938064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83870235"/>
+        <c:axId val="52901568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3117,7 +2787,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86159457"/>
+        <c:crossAx val="2938064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3125,7 +2795,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86159457"/>
+        <c:axId val="2938064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3199,7 +2869,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83870235"/>
+        <c:crossAx val="52901568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3219,14 +2889,14 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3272,10 +2942,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0822335657370518"/>
-          <c:y val="0.161875945537065"/>
-          <c:w val="0.88433764940239"/>
-          <c:h val="0.63565305093293"/>
+          <c:x val="0.0822386851771151"/>
+          <c:y val="0.161896356071113"/>
+          <c:w val="0.884268193986179"/>
+          <c:h val="0.635607111335267"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3384,11 +3054,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="56381240"/>
-        <c:axId val="32729073"/>
+        <c:axId val="41609785"/>
+        <c:axId val="34076427"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="56381240"/>
+        <c:axId val="41609785"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -3455,12 +3125,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32729073"/>
+        <c:crossAx val="34076427"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="32729073"/>
+        <c:axId val="34076427"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -3535,7 +3205,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56381240"/>
+        <c:crossAx val="41609785"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3555,7 +3225,343 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Product Backlog Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0821883587309518"/>
+          <c:y val="0.161896356071113"/>
+          <c:w val="0.88427429427929"/>
+          <c:h val="0.635607111335267"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="line"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Product Backlog'!$A$12:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Product Backlog'!$B$12:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="8529643"/>
+        <c:axId val="56826859"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="8529643"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="6"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Sprints</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="56826859"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="56826859"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Features Remaining at end of Sprint</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="8529643"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -3573,9 +3579,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>3702600</xdr:colOff>
+      <xdr:colOff>3702240</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>120240</xdr:rowOff>
+      <xdr:rowOff>119880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3583,8 +3589,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9114840" y="267840"/>
-        <a:ext cx="5764320" cy="2855160"/>
+        <a:off x="9112680" y="267840"/>
+        <a:ext cx="5763960" cy="2854800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3608,9 +3614,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3618,8 +3624,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="553680"/>
-        <a:ext cx="3747240" cy="1847520"/>
+        <a:off x="4090680" y="553680"/>
+        <a:ext cx="3747600" cy="1847160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3643,9 +3649,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3653,8 +3659,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="553680"/>
-        <a:ext cx="3747240" cy="1847520"/>
+        <a:off x="4090680" y="553680"/>
+        <a:ext cx="3747600" cy="1847160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3678,9 +3684,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3688,8 +3694,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="553680"/>
-        <a:ext cx="3747240" cy="1847520"/>
+        <a:off x="4090680" y="553680"/>
+        <a:ext cx="3747600" cy="1847160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3713,9 +3719,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3723,8 +3729,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="553680"/>
-        <a:ext cx="3747240" cy="1847520"/>
+        <a:off x="4090680" y="553680"/>
+        <a:ext cx="3747600" cy="1847160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3748,9 +3754,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3758,8 +3764,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="553680"/>
-        <a:ext cx="3747240" cy="1847520"/>
+        <a:off x="4090680" y="553680"/>
+        <a:ext cx="3747600" cy="1847160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3783,9 +3789,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3793,8 +3799,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="553680"/>
-        <a:ext cx="3747240" cy="1847520"/>
+        <a:off x="4090680" y="553680"/>
+        <a:ext cx="3747600" cy="1847160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3818,9 +3824,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>3790080</xdr:colOff>
+      <xdr:colOff>3789720</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>120240</xdr:rowOff>
+      <xdr:rowOff>119880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3828,8 +3834,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9113400" y="267840"/>
-        <a:ext cx="5782680" cy="2855160"/>
+        <a:off x="9111960" y="267840"/>
+        <a:ext cx="5782320" cy="2854800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3850,8 +3856,8 @@
   </sheetPr>
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H44" activeCellId="0" sqref="H44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I41" activeCellId="0" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3860,7 +3866,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="4.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="45.57"/>
@@ -4098,11 +4104,11 @@
       </c>
       <c r="B17" s="3" t="n">
         <f aca="false">B16-C17</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="10" t="n">
         <f aca="false">COUNTIF(F$24:F$67,"Finished in Sprint 5")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="12"/>
@@ -4117,7 +4123,7 @@
       </c>
       <c r="B18" s="3" t="n">
         <f aca="false">B17-C18</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="10" t="n">
         <f aca="false">COUNTIF(F$24:F$67,"Finished in Sprint 6")</f>
@@ -4603,22 +4609,26 @@
       <c r="D36" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="E36" s="17"/>
-      <c r="F36" s="18"/>
+      <c r="E36" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="F36" s="18" t="s">
+        <v>80</v>
+      </c>
       <c r="G36" s="14" t="s">
         <v>76</v>
       </c>
       <c r="H36" s="19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I36" s="19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J36" s="19"/>
     </row>
     <row r="37" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B37" s="11" t="n">
         <v>14</v>
@@ -4629,24 +4639,28 @@
       <c r="D37" s="11" t="n">
         <v>8</v>
       </c>
-      <c r="E37" s="17"/>
-      <c r="F37" s="18"/>
+      <c r="E37" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="F37" s="18" t="s">
+        <v>84</v>
+      </c>
       <c r="G37" s="14" t="s">
         <v>76</v>
       </c>
       <c r="H37" s="19" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I37" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="J37" s="19" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B38" s="11" t="n">
         <v>15</v>
@@ -4657,24 +4671,28 @@
       <c r="D38" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="E38" s="17"/>
-      <c r="F38" s="18"/>
+      <c r="E38" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>84</v>
+      </c>
       <c r="G38" s="14" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H38" s="19" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I38" s="19" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J38" s="19" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" s="24" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B39" s="11" t="n">
         <v>16</v>
@@ -4685,24 +4703,28 @@
       <c r="D39" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="E39" s="17"/>
-      <c r="F39" s="18"/>
+      <c r="E39" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>84</v>
+      </c>
       <c r="G39" s="14" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H39" s="19" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I39" s="19" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="J39" s="19" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" s="24" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B40" s="11" t="n">
         <v>17</v>
@@ -4713,24 +4735,28 @@
       <c r="D40" s="11" t="n">
         <v>8</v>
       </c>
-      <c r="E40" s="17"/>
-      <c r="F40" s="18"/>
+      <c r="E40" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>84</v>
+      </c>
       <c r="G40" s="14" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H40" s="19" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="I40" s="19" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="J40" s="19" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" s="24" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B41" s="11" t="n">
         <v>18</v>
@@ -4741,24 +4767,28 @@
       <c r="D41" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="E41" s="17"/>
-      <c r="F41" s="18"/>
+      <c r="E41" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="F41" s="18" t="s">
+        <v>84</v>
+      </c>
       <c r="G41" s="14" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H41" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="I41" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="J41" s="19" t="s">
         <v>100</v>
-      </c>
-      <c r="I41" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="J41" s="19" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="42" s="26" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="20" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B42" s="21" t="n">
         <v>19</v>
@@ -4775,18 +4805,18 @@
         <v>36</v>
       </c>
       <c r="H42" s="23" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I42" s="23" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J42" s="23" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="20" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B43" s="21" t="n">
         <v>20</v>
@@ -4803,18 +4833,18 @@
         <v>36</v>
       </c>
       <c r="H43" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="I43" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="J43" s="23" t="s">
         <v>107</v>
-      </c>
-      <c r="I43" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="J43" s="23" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="20" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B44" s="21" t="n">
         <v>21</v>
@@ -4831,10 +4861,10 @@
         <v>36</v>
       </c>
       <c r="H44" s="23" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I44" s="23" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="J44" s="23"/>
     </row>
@@ -4856,7 +4886,7 @@
       <c r="E46" s="11"/>
       <c r="F46" s="11"/>
       <c r="G46" s="13" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H46" s="19"/>
       <c r="I46" s="19"/>
@@ -4865,13 +4895,13 @@
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="11"/>
       <c r="C47" s="16" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D47" s="11"/>
       <c r="E47" s="11"/>
       <c r="F47" s="11"/>
       <c r="G47" s="14" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H47" s="19"/>
       <c r="I47" s="19"/>
@@ -4879,7 +4909,7 @@
     </row>
     <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B48" s="11" t="n">
         <v>22</v>
@@ -4893,21 +4923,21 @@
       <c r="E48" s="17"/>
       <c r="F48" s="18"/>
       <c r="G48" s="14" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H48" s="19" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I48" s="19" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="J48" s="19" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B49" s="11" t="n">
         <v>23</v>
@@ -4924,16 +4954,16 @@
         <v>64</v>
       </c>
       <c r="H49" s="19" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="I49" s="19" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="J49" s="19"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B50" s="11" t="n">
         <v>24</v>
@@ -4950,16 +4980,16 @@
         <v>36</v>
       </c>
       <c r="H50" s="19" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="I50" s="19" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="J50" s="19"/>
     </row>
     <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B51" s="11" t="n">
         <v>25</v>
@@ -4976,16 +5006,16 @@
         <v>36</v>
       </c>
       <c r="H51" s="19" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I51" s="19" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="J51" s="19"/>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B52" s="11" t="n">
         <v>26</v>
@@ -5002,16 +5032,16 @@
         <v>36</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I52" s="19" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="J52" s="19"/>
     </row>
     <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B53" s="11" t="n">
         <v>27</v>
@@ -5028,16 +5058,16 @@
         <v>76</v>
       </c>
       <c r="H53" s="19" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="I53" s="19" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J53" s="19"/>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B54" s="11" t="n">
         <v>28</v>
@@ -5054,16 +5084,16 @@
         <v>76</v>
       </c>
       <c r="H54" s="19" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="I54" s="19" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="J54" s="19"/>
     </row>
     <row r="55" s="24" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B55" s="11" t="n">
         <v>29</v>
@@ -5080,18 +5110,18 @@
         <v>36</v>
       </c>
       <c r="H55" s="19" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="I55" s="19" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="J55" s="19" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="56" s="24" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B56" s="11" t="n">
         <v>30</v>
@@ -5108,18 +5138,18 @@
         <v>76</v>
       </c>
       <c r="H56" s="19" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="I56" s="19" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="J56" s="19" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B57" s="11" t="n">
         <v>31</v>
@@ -5136,16 +5166,16 @@
         <v>36</v>
       </c>
       <c r="H57" s="19" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I57" s="19" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="J57" s="19"/>
     </row>
     <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B58" s="11" t="n">
         <v>32</v>
@@ -5162,16 +5192,16 @@
         <v>36</v>
       </c>
       <c r="H58" s="19" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I58" s="19" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="J58" s="19"/>
     </row>
     <row r="59" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B59" s="11" t="n">
         <v>33</v>
@@ -5188,16 +5218,16 @@
         <v>36</v>
       </c>
       <c r="H59" s="19" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I59" s="19" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="J59" s="19"/>
     </row>
     <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B60" s="11" t="n">
         <v>34</v>
@@ -5214,16 +5244,16 @@
         <v>36</v>
       </c>
       <c r="H60" s="19" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="I60" s="19" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="J60" s="19"/>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B61" s="11" t="n">
         <v>35</v>
@@ -5240,7 +5270,7 @@
         <v>64</v>
       </c>
       <c r="H61" s="19" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I61" s="19" t="s">
         <v>66</v>
@@ -5249,7 +5279,7 @@
     </row>
     <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B62" s="11" t="n">
         <v>36</v>
@@ -5266,10 +5296,10 @@
         <v>36</v>
       </c>
       <c r="H62" s="19" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="I62" s="19" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="J62" s="19"/>
     </row>
@@ -5344,7 +5374,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -5368,21 +5398,21 @@
     </row>
     <row r="2" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="27" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B2" s="30" t="n">
         <v>44474</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="31" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E2" s="27"/>
       <c r="F2" s="27"/>
     </row>
     <row r="3" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="27" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B3" s="30" t="n">
         <f aca="false">B2+7</f>
@@ -5395,10 +5425,10 @@
     </row>
     <row r="4" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="27" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
@@ -5419,7 +5449,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="27"/>
@@ -5427,7 +5457,7 @@
     </row>
     <row r="7" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="27" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B7" s="27" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
@@ -5440,7 +5470,7 @@
     </row>
     <row r="8" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="27" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B8" s="27" t="n">
         <f aca="false">B7-C8</f>
@@ -5456,7 +5486,7 @@
     </row>
     <row r="9" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="27" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B9" s="27" t="n">
         <f aca="false">B8-C9</f>
@@ -5472,7 +5502,7 @@
     </row>
     <row r="10" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="27" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B10" s="27" t="n">
         <f aca="false">B9-C10</f>
@@ -5488,7 +5518,7 @@
     </row>
     <row r="11" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="27" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B11" s="27" t="n">
         <f aca="false">B10-C11</f>
@@ -5504,7 +5534,7 @@
     </row>
     <row r="12" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="27" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B12" s="27" t="n">
         <f aca="false">B11-C12</f>
@@ -5520,7 +5550,7 @@
     </row>
     <row r="13" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="27" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B13" s="27" t="n">
         <f aca="false">B12-C13</f>
@@ -5536,7 +5566,7 @@
     </row>
     <row r="14" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="27" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B14" s="27" t="n">
         <f aca="false">B13-C14</f>
@@ -5560,16 +5590,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="34" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B16" s="34" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E16" s="34" t="s">
         <v>29</v>
@@ -5584,7 +5614,7 @@
       </c>
       <c r="B17" s="35"/>
       <c r="D17" s="36" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E17" s="37"/>
     </row>
@@ -6301,7 +6331,7 @@
       <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -6326,7 +6356,7 @@
     </row>
     <row r="2" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="27" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B2" s="30" t="n">
         <f aca="false">'Sprint 01 Backlog'!B3</f>
@@ -6334,14 +6364,14 @@
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="31" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E2" s="27"/>
       <c r="F2" s="27"/>
     </row>
     <row r="3" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="27" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B3" s="30" t="n">
         <f aca="false">B2+7</f>
@@ -6354,10 +6384,10 @@
     </row>
     <row r="4" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="27" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
@@ -6378,7 +6408,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="27"/>
@@ -6386,7 +6416,7 @@
     </row>
     <row r="7" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="27" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B7" s="27" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
@@ -6399,7 +6429,7 @@
     </row>
     <row r="8" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="27" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B8" s="27" t="n">
         <f aca="false">B7-C8</f>
@@ -6415,7 +6445,7 @@
     </row>
     <row r="9" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="27" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B9" s="27" t="n">
         <f aca="false">B8-C9</f>
@@ -6431,7 +6461,7 @@
     </row>
     <row r="10" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="27" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B10" s="27" t="n">
         <f aca="false">B9-C10</f>
@@ -6447,7 +6477,7 @@
     </row>
     <row r="11" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="27" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B11" s="27" t="n">
         <f aca="false">B10-C11</f>
@@ -6463,7 +6493,7 @@
     </row>
     <row r="12" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="27" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B12" s="27" t="n">
         <f aca="false">B11-C12</f>
@@ -6479,7 +6509,7 @@
     </row>
     <row r="13" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="27" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B13" s="27" t="n">
         <f aca="false">B12-C13</f>
@@ -6495,7 +6525,7 @@
     </row>
     <row r="14" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="27" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B14" s="27" t="n">
         <f aca="false">B13-C14</f>
@@ -6519,16 +6549,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="34" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B16" s="34" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E16" s="34" t="s">
         <v>29</v>
@@ -6545,10 +6575,10 @@
         <v>45</v>
       </c>
       <c r="D17" s="36" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E17" s="39" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6562,7 +6592,7 @@
         <v>51</v>
       </c>
       <c r="E18" s="39" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7270,7 +7300,7 @@
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -7295,7 +7325,7 @@
     </row>
     <row r="2" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="27" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B2" s="30" t="n">
         <f aca="false">'Sprint 02 Backlog'!B3</f>
@@ -7303,14 +7333,14 @@
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="31" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E2" s="27"/>
       <c r="F2" s="27"/>
     </row>
     <row r="3" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="27" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B3" s="30" t="n">
         <f aca="false">B2+7</f>
@@ -7323,10 +7353,10 @@
     </row>
     <row r="4" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="27" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
@@ -7347,7 +7377,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="27"/>
@@ -7355,7 +7385,7 @@
     </row>
     <row r="7" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="27" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B7" s="27" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
@@ -7368,7 +7398,7 @@
     </row>
     <row r="8" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="27" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B8" s="27" t="n">
         <f aca="false">B7-C8</f>
@@ -7384,7 +7414,7 @@
     </row>
     <row r="9" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="27" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B9" s="27" t="n">
         <f aca="false">B8-C9</f>
@@ -7400,7 +7430,7 @@
     </row>
     <row r="10" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="27" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B10" s="27" t="n">
         <f aca="false">B9-C10</f>
@@ -7416,7 +7446,7 @@
     </row>
     <row r="11" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="27" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B11" s="27" t="n">
         <f aca="false">B10-C11</f>
@@ -7432,7 +7462,7 @@
     </row>
     <row r="12" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="27" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B12" s="27" t="n">
         <f aca="false">B11-C12</f>
@@ -7448,7 +7478,7 @@
     </row>
     <row r="13" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="27" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B13" s="27" t="n">
         <f aca="false">B12-C13</f>
@@ -7464,7 +7494,7 @@
     </row>
     <row r="14" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="27" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B14" s="27" t="n">
         <f aca="false">B13-C14</f>
@@ -7488,16 +7518,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="34" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B16" s="34" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E16" s="34" t="s">
         <v>29</v>
@@ -7514,10 +7544,10 @@
         <v>53</v>
       </c>
       <c r="D17" s="36" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E17" s="39" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7528,10 +7558,10 @@
         <v>58</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E18" s="39" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7542,10 +7572,10 @@
         <v>61</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="E19" s="39" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7556,10 +7586,10 @@
         <v>63</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E20" s="39" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7570,10 +7600,10 @@
         <v>68</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E21" s="39" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8257,7 +8287,7 @@
       <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -8282,21 +8312,21 @@
     </row>
     <row r="2" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="27" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B2" s="30" t="n">
         <v>44502</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="31" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E2" s="27"/>
       <c r="F2" s="27"/>
     </row>
     <row r="3" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="27" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B3" s="30" t="n">
         <f aca="false">B2+7</f>
@@ -8309,10 +8339,10 @@
     </row>
     <row r="4" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="27" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
@@ -8333,7 +8363,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="27"/>
@@ -8341,7 +8371,7 @@
     </row>
     <row r="7" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="27" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B7" s="27" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
@@ -8354,7 +8384,7 @@
     </row>
     <row r="8" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="27" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B8" s="27" t="n">
         <f aca="false">B7-C8</f>
@@ -8370,7 +8400,7 @@
     </row>
     <row r="9" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="27" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B9" s="27" t="n">
         <f aca="false">B8-C9</f>
@@ -8386,7 +8416,7 @@
     </row>
     <row r="10" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="27" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B10" s="27" t="n">
         <f aca="false">B9-C10</f>
@@ -8402,7 +8432,7 @@
     </row>
     <row r="11" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="27" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B11" s="27" t="n">
         <f aca="false">B10-C11</f>
@@ -8418,7 +8448,7 @@
     </row>
     <row r="12" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="27" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B12" s="27" t="n">
         <f aca="false">B11-C12</f>
@@ -8434,7 +8464,7 @@
     </row>
     <row r="13" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="27" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B13" s="27" t="n">
         <f aca="false">B12-C13</f>
@@ -8450,7 +8480,7 @@
     </row>
     <row r="14" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="27" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B14" s="27" t="n">
         <f aca="false">B13-C14</f>
@@ -8474,16 +8504,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="34" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B16" s="34" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E16" s="34" t="s">
         <v>29</v>
@@ -8500,10 +8530,10 @@
         <v>75</v>
       </c>
       <c r="D17" s="36" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E17" s="39" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8514,10 +8544,10 @@
         <v>70</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E18" s="39" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9221,11 +9251,11 @@
   </sheetPr>
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -9250,7 +9280,7 @@
     </row>
     <row r="2" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="27" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B2" s="30" t="n">
         <f aca="false">'Sprint 04 Backlog'!B3</f>
@@ -9258,14 +9288,14 @@
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="31" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E2" s="27"/>
       <c r="F2" s="27"/>
     </row>
     <row r="3" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="27" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B3" s="30" t="n">
         <f aca="false">B2+7</f>
@@ -9278,10 +9308,10 @@
     </row>
     <row r="4" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="27" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
@@ -9302,7 +9332,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="27"/>
@@ -9310,7 +9340,7 @@
     </row>
     <row r="7" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="27" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B7" s="27" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
@@ -9323,7 +9353,7 @@
     </row>
     <row r="8" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="27" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B8" s="27" t="n">
         <f aca="false">B7-C8</f>
@@ -9339,7 +9369,7 @@
     </row>
     <row r="9" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="27" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B9" s="27" t="n">
         <f aca="false">B8-C9</f>
@@ -9355,7 +9385,7 @@
     </row>
     <row r="10" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="27" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B10" s="27" t="n">
         <f aca="false">B9-C10</f>
@@ -9371,7 +9401,7 @@
     </row>
     <row r="11" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="27" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B11" s="27" t="n">
         <f aca="false">B10-C11</f>
@@ -9387,7 +9417,7 @@
     </row>
     <row r="12" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="27" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B12" s="27" t="n">
         <f aca="false">B11-C12</f>
@@ -9403,7 +9433,7 @@
     </row>
     <row r="13" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="27" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B13" s="27" t="n">
         <f aca="false">B12-C13</f>
@@ -9419,15 +9449,15 @@
     </row>
     <row r="14" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="27" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B14" s="27" t="n">
         <f aca="false">B13-C14</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="27" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 7")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="27"/>
       <c r="E14" s="27"/>
@@ -9443,16 +9473,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="34" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B16" s="34" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E16" s="34" t="s">
         <v>29</v>
@@ -9465,675 +9495,695 @@
       <c r="A17" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B17" s="35"/>
+      <c r="B17" s="38" t="s">
+        <v>79</v>
+      </c>
       <c r="D17" s="36" t="s">
-        <v>179</v>
-      </c>
-      <c r="E17" s="37"/>
+        <v>181</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B18" s="35"/>
+      <c r="B18" s="38" t="s">
+        <v>83</v>
+      </c>
       <c r="D18" s="35"/>
-      <c r="E18" s="37"/>
+      <c r="E18" s="39" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B19" s="35"/>
+      <c r="B19" s="38" t="s">
+        <v>88</v>
+      </c>
       <c r="D19" s="35"/>
-      <c r="E19" s="37"/>
+      <c r="E19" s="39" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B20" s="35"/>
+      <c r="B20" s="38" t="s">
+        <v>93</v>
+      </c>
       <c r="D20" s="35"/>
-      <c r="E20" s="37"/>
+      <c r="E20" s="39" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B21" s="35"/>
+      <c r="B21" s="38" t="s">
+        <v>97</v>
+      </c>
       <c r="D21" s="35"/>
-      <c r="E21" s="37"/>
+      <c r="E21" s="39" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B22" s="35"/>
+      <c r="B22" s="38"/>
       <c r="D22" s="35"/>
-      <c r="E22" s="37"/>
+      <c r="E22" s="39"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B23" s="35"/>
+      <c r="B23" s="38"/>
       <c r="D23" s="35"/>
-      <c r="E23" s="37"/>
+      <c r="E23" s="39"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B24" s="35"/>
+      <c r="B24" s="38"/>
       <c r="D24" s="35"/>
-      <c r="E24" s="37"/>
+      <c r="E24" s="39"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="B25" s="35"/>
+      <c r="B25" s="38"/>
       <c r="D25" s="35"/>
-      <c r="E25" s="37"/>
+      <c r="E25" s="39"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B26" s="35"/>
+      <c r="B26" s="38"/>
       <c r="D26" s="35"/>
-      <c r="E26" s="37"/>
+      <c r="E26" s="39"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="B27" s="35"/>
+      <c r="B27" s="38"/>
       <c r="D27" s="35"/>
-      <c r="E27" s="37"/>
+      <c r="E27" s="39"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="B28" s="35"/>
+      <c r="B28" s="38"/>
       <c r="D28" s="35"/>
-      <c r="E28" s="37"/>
+      <c r="E28" s="39"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="B29" s="35"/>
+      <c r="B29" s="38"/>
       <c r="D29" s="35"/>
-      <c r="E29" s="37"/>
+      <c r="E29" s="39"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B30" s="35"/>
+      <c r="B30" s="38"/>
       <c r="D30" s="35"/>
-      <c r="E30" s="37"/>
+      <c r="E30" s="39"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B31" s="35"/>
+      <c r="B31" s="38"/>
       <c r="D31" s="35"/>
-      <c r="E31" s="37"/>
+      <c r="E31" s="39"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="B32" s="35"/>
+      <c r="B32" s="38"/>
       <c r="D32" s="35"/>
-      <c r="E32" s="37"/>
+      <c r="E32" s="39"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="B33" s="35"/>
+      <c r="B33" s="38"/>
       <c r="D33" s="35"/>
-      <c r="E33" s="37"/>
+      <c r="E33" s="39"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="B34" s="35"/>
+      <c r="B34" s="38"/>
       <c r="D34" s="35"/>
-      <c r="E34" s="37"/>
+      <c r="E34" s="39"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="B35" s="35"/>
+      <c r="B35" s="38"/>
       <c r="D35" s="35"/>
-      <c r="E35" s="37"/>
+      <c r="E35" s="39"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B36" s="35"/>
+      <c r="B36" s="38"/>
       <c r="D36" s="35"/>
-      <c r="E36" s="37"/>
+      <c r="E36" s="39"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="B37" s="35"/>
+      <c r="B37" s="38"/>
       <c r="D37" s="35"/>
-      <c r="E37" s="37"/>
+      <c r="E37" s="39"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="B38" s="35"/>
+      <c r="B38" s="38"/>
       <c r="D38" s="35"/>
-      <c r="E38" s="37"/>
+      <c r="E38" s="39"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="B39" s="35"/>
+      <c r="B39" s="38"/>
       <c r="D39" s="35"/>
-      <c r="E39" s="37"/>
+      <c r="E39" s="39"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B40" s="35"/>
+      <c r="B40" s="38"/>
       <c r="D40" s="35"/>
-      <c r="E40" s="37"/>
+      <c r="E40" s="39"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B41" s="35"/>
+      <c r="B41" s="38"/>
       <c r="D41" s="35"/>
-      <c r="E41" s="37"/>
+      <c r="E41" s="39"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="B42" s="35"/>
+      <c r="B42" s="38"/>
       <c r="D42" s="35"/>
-      <c r="E42" s="37"/>
+      <c r="E42" s="39"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="B43" s="35"/>
+      <c r="B43" s="38"/>
       <c r="D43" s="35"/>
-      <c r="E43" s="37"/>
+      <c r="E43" s="39"/>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="B44" s="35"/>
+      <c r="B44" s="38"/>
       <c r="D44" s="35"/>
-      <c r="E44" s="37"/>
+      <c r="E44" s="39"/>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="B45" s="35"/>
+      <c r="B45" s="38"/>
       <c r="D45" s="35"/>
-      <c r="E45" s="37"/>
+      <c r="E45" s="39"/>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B46" s="35"/>
+      <c r="B46" s="38"/>
       <c r="D46" s="35"/>
-      <c r="E46" s="37"/>
+      <c r="E46" s="39"/>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="B47" s="35"/>
+      <c r="B47" s="38"/>
       <c r="D47" s="35"/>
-      <c r="E47" s="37"/>
+      <c r="E47" s="39"/>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B48" s="35"/>
+      <c r="B48" s="38"/>
       <c r="D48" s="35"/>
-      <c r="E48" s="37"/>
+      <c r="E48" s="39"/>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="B49" s="35"/>
+      <c r="B49" s="38"/>
       <c r="D49" s="35"/>
-      <c r="E49" s="37"/>
+      <c r="E49" s="39"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="B50" s="35"/>
+      <c r="B50" s="38"/>
       <c r="D50" s="35"/>
-      <c r="E50" s="37"/>
+      <c r="E50" s="39"/>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="B51" s="35"/>
+      <c r="B51" s="38"/>
       <c r="D51" s="35"/>
-      <c r="E51" s="37"/>
+      <c r="E51" s="39"/>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="B52" s="35"/>
+      <c r="B52" s="38"/>
       <c r="D52" s="35"/>
-      <c r="E52" s="37"/>
+      <c r="E52" s="39"/>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="B53" s="35"/>
+      <c r="B53" s="38"/>
       <c r="D53" s="35"/>
-      <c r="E53" s="37"/>
+      <c r="E53" s="39"/>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="B54" s="35"/>
+      <c r="B54" s="38"/>
       <c r="D54" s="35"/>
-      <c r="E54" s="37"/>
+      <c r="E54" s="39"/>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="B55" s="35"/>
+      <c r="B55" s="38"/>
       <c r="D55" s="35"/>
-      <c r="E55" s="37"/>
+      <c r="E55" s="39"/>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="B56" s="35"/>
+      <c r="B56" s="38"/>
       <c r="D56" s="35"/>
-      <c r="E56" s="37"/>
+      <c r="E56" s="39"/>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="B57" s="35"/>
+      <c r="B57" s="38"/>
       <c r="D57" s="35"/>
-      <c r="E57" s="37"/>
+      <c r="E57" s="39"/>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="B58" s="35"/>
+      <c r="B58" s="38"/>
       <c r="D58" s="35"/>
-      <c r="E58" s="37"/>
+      <c r="E58" s="39"/>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
         <v>43</v>
       </c>
-      <c r="B59" s="35"/>
+      <c r="B59" s="38"/>
       <c r="D59" s="35"/>
-      <c r="E59" s="37"/>
+      <c r="E59" s="39"/>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="B60" s="35"/>
+      <c r="B60" s="38"/>
       <c r="D60" s="35"/>
-      <c r="E60" s="37"/>
+      <c r="E60" s="39"/>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="B61" s="35"/>
+      <c r="B61" s="38"/>
       <c r="D61" s="35"/>
-      <c r="E61" s="37"/>
+      <c r="E61" s="39"/>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
         <v>46</v>
       </c>
-      <c r="B62" s="35"/>
+      <c r="B62" s="38"/>
       <c r="D62" s="35"/>
-      <c r="E62" s="37"/>
+      <c r="E62" s="39"/>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="B63" s="35"/>
+      <c r="B63" s="38"/>
       <c r="D63" s="35"/>
-      <c r="E63" s="37"/>
+      <c r="E63" s="39"/>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="B64" s="35"/>
+      <c r="B64" s="38"/>
       <c r="D64" s="35"/>
-      <c r="E64" s="37"/>
+      <c r="E64" s="39"/>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="B65" s="35"/>
+      <c r="B65" s="38"/>
       <c r="D65" s="35"/>
-      <c r="E65" s="37"/>
+      <c r="E65" s="39"/>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="B66" s="35"/>
+      <c r="B66" s="38"/>
       <c r="D66" s="35"/>
-      <c r="E66" s="37"/>
+      <c r="E66" s="39"/>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
         <v>51</v>
       </c>
-      <c r="B67" s="35"/>
+      <c r="B67" s="38"/>
       <c r="D67" s="35"/>
-      <c r="E67" s="37"/>
+      <c r="E67" s="39"/>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
         <v>52</v>
       </c>
-      <c r="B68" s="35"/>
+      <c r="B68" s="38"/>
       <c r="D68" s="35"/>
-      <c r="E68" s="37"/>
+      <c r="E68" s="39"/>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
         <v>53</v>
       </c>
-      <c r="B69" s="35"/>
+      <c r="B69" s="38"/>
       <c r="D69" s="35"/>
-      <c r="E69" s="37"/>
+      <c r="E69" s="39"/>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
         <v>54</v>
       </c>
-      <c r="B70" s="35"/>
+      <c r="B70" s="38"/>
       <c r="D70" s="35"/>
-      <c r="E70" s="37"/>
+      <c r="E70" s="39"/>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="B71" s="35"/>
+      <c r="B71" s="38"/>
       <c r="D71" s="35"/>
-      <c r="E71" s="37"/>
+      <c r="E71" s="39"/>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
         <v>56</v>
       </c>
-      <c r="B72" s="35"/>
+      <c r="B72" s="38"/>
       <c r="D72" s="35"/>
-      <c r="E72" s="37"/>
+      <c r="E72" s="39"/>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
         <v>57</v>
       </c>
-      <c r="B73" s="35"/>
+      <c r="B73" s="38"/>
       <c r="D73" s="35"/>
-      <c r="E73" s="37"/>
+      <c r="E73" s="39"/>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
         <v>58</v>
       </c>
-      <c r="B74" s="35"/>
+      <c r="B74" s="38"/>
       <c r="D74" s="35"/>
-      <c r="E74" s="37"/>
+      <c r="E74" s="39"/>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="B75" s="35"/>
+      <c r="B75" s="38"/>
       <c r="D75" s="35"/>
-      <c r="E75" s="37"/>
+      <c r="E75" s="39"/>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="B76" s="35"/>
+      <c r="B76" s="38"/>
       <c r="D76" s="35"/>
-      <c r="E76" s="37"/>
+      <c r="E76" s="39"/>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
         <v>61</v>
       </c>
-      <c r="B77" s="35"/>
+      <c r="B77" s="38"/>
       <c r="D77" s="35"/>
-      <c r="E77" s="37"/>
+      <c r="E77" s="39"/>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
         <v>62</v>
       </c>
-      <c r="B78" s="35"/>
+      <c r="B78" s="38"/>
       <c r="D78" s="35"/>
-      <c r="E78" s="37"/>
+      <c r="E78" s="39"/>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
         <v>63</v>
       </c>
-      <c r="B79" s="35"/>
+      <c r="B79" s="38"/>
       <c r="D79" s="35"/>
-      <c r="E79" s="37"/>
+      <c r="E79" s="39"/>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
         <v>64</v>
       </c>
-      <c r="B80" s="35"/>
+      <c r="B80" s="38"/>
       <c r="D80" s="35"/>
-      <c r="E80" s="37"/>
+      <c r="E80" s="39"/>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="B81" s="35"/>
+      <c r="B81" s="38"/>
       <c r="D81" s="35"/>
-      <c r="E81" s="37"/>
+      <c r="E81" s="39"/>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
         <v>66</v>
       </c>
-      <c r="B82" s="35"/>
+      <c r="B82" s="38"/>
       <c r="D82" s="35"/>
-      <c r="E82" s="37"/>
+      <c r="E82" s="39"/>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="B83" s="35"/>
+      <c r="B83" s="38"/>
       <c r="D83" s="35"/>
-      <c r="E83" s="37"/>
+      <c r="E83" s="39"/>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
         <v>68</v>
       </c>
-      <c r="B84" s="35"/>
+      <c r="B84" s="38"/>
       <c r="D84" s="35"/>
-      <c r="E84" s="37"/>
+      <c r="E84" s="39"/>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="n">
         <v>69</v>
       </c>
-      <c r="B85" s="35"/>
+      <c r="B85" s="38"/>
       <c r="D85" s="35"/>
-      <c r="E85" s="37"/>
+      <c r="E85" s="39"/>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="B86" s="35"/>
+      <c r="B86" s="38"/>
       <c r="D86" s="35"/>
-      <c r="E86" s="37"/>
+      <c r="E86" s="39"/>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="B87" s="35"/>
+      <c r="B87" s="38"/>
       <c r="D87" s="35"/>
-      <c r="E87" s="37"/>
+      <c r="E87" s="39"/>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="n">
         <v>72</v>
       </c>
-      <c r="B88" s="35"/>
+      <c r="B88" s="38"/>
       <c r="D88" s="35"/>
-      <c r="E88" s="37"/>
+      <c r="E88" s="39"/>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="n">
         <v>73</v>
       </c>
-      <c r="B89" s="35"/>
+      <c r="B89" s="38"/>
       <c r="D89" s="35"/>
-      <c r="E89" s="37"/>
+      <c r="E89" s="39"/>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="n">
         <v>74</v>
       </c>
-      <c r="B90" s="35"/>
+      <c r="B90" s="38"/>
       <c r="D90" s="35"/>
-      <c r="E90" s="37"/>
+      <c r="E90" s="39"/>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="n">
         <v>75</v>
       </c>
-      <c r="B91" s="35"/>
+      <c r="B91" s="38"/>
       <c r="D91" s="35"/>
-      <c r="E91" s="37"/>
+      <c r="E91" s="39"/>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="n">
         <v>76</v>
       </c>
-      <c r="B92" s="35"/>
+      <c r="B92" s="38"/>
       <c r="D92" s="35"/>
-      <c r="E92" s="37"/>
+      <c r="E92" s="39"/>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="n">
         <v>77</v>
       </c>
-      <c r="B93" s="35"/>
+      <c r="B93" s="38"/>
       <c r="D93" s="35"/>
-      <c r="E93" s="37"/>
+      <c r="E93" s="39"/>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="n">
         <v>78</v>
       </c>
-      <c r="B94" s="35"/>
+      <c r="B94" s="38"/>
       <c r="D94" s="35"/>
-      <c r="E94" s="37"/>
+      <c r="E94" s="39"/>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="n">
         <v>79</v>
       </c>
-      <c r="B95" s="35"/>
+      <c r="B95" s="38"/>
       <c r="D95" s="35"/>
-      <c r="E95" s="37"/>
+      <c r="E95" s="39"/>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="B96" s="35"/>
+      <c r="B96" s="38"/>
       <c r="D96" s="35"/>
-      <c r="E96" s="37"/>
+      <c r="E96" s="39"/>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="n">
         <v>81</v>
       </c>
-      <c r="B97" s="35"/>
+      <c r="B97" s="38"/>
       <c r="D97" s="35"/>
-      <c r="E97" s="37"/>
+      <c r="E97" s="39"/>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="n">
         <v>82</v>
       </c>
-      <c r="B98" s="35"/>
+      <c r="B98" s="38"/>
       <c r="D98" s="35"/>
-      <c r="E98" s="37"/>
+      <c r="E98" s="39"/>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="n">
         <v>83</v>
       </c>
-      <c r="B99" s="35"/>
+      <c r="B99" s="38"/>
       <c r="D99" s="35"/>
-      <c r="E99" s="37"/>
+      <c r="E99" s="39"/>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="n">
         <v>84</v>
       </c>
-      <c r="B100" s="35"/>
+      <c r="B100" s="38"/>
       <c r="D100" s="35"/>
-      <c r="E100" s="37"/>
+      <c r="E100" s="39"/>
     </row>
   </sheetData>
   <dataValidations count="6">
@@ -10184,7 +10234,7 @@
       <selection pane="topLeft" activeCell="G40" activeCellId="0" sqref="G40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -10209,21 +10259,21 @@
     </row>
     <row r="2" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="27" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B2" s="30" t="n">
         <v>44530</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="31" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E2" s="27"/>
       <c r="F2" s="27"/>
     </row>
     <row r="3" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="27" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B3" s="30" t="n">
         <f aca="false">B2+7</f>
@@ -10231,17 +10281,17 @@
       </c>
       <c r="C3" s="27"/>
       <c r="D3" s="40" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E3" s="27"/>
       <c r="F3" s="27"/>
     </row>
     <row r="4" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="27" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
@@ -10262,7 +10312,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="27"/>
@@ -10270,7 +10320,7 @@
     </row>
     <row r="7" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="27" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B7" s="27" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
@@ -10283,7 +10333,7 @@
     </row>
     <row r="8" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="27" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B8" s="27" t="n">
         <f aca="false">B7-C8</f>
@@ -10299,7 +10349,7 @@
     </row>
     <row r="9" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="27" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B9" s="27" t="n">
         <f aca="false">B8-C9</f>
@@ -10315,7 +10365,7 @@
     </row>
     <row r="10" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="27" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B10" s="27" t="n">
         <f aca="false">B9-C10</f>
@@ -10331,7 +10381,7 @@
     </row>
     <row r="11" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="27" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B11" s="27" t="n">
         <f aca="false">B10-C11</f>
@@ -10347,7 +10397,7 @@
     </row>
     <row r="12" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="27" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B12" s="27" t="n">
         <f aca="false">B11-C12</f>
@@ -10363,7 +10413,7 @@
     </row>
     <row r="13" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="27" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B13" s="27" t="n">
         <f aca="false">B12-C13</f>
@@ -10379,7 +10429,7 @@
     </row>
     <row r="14" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="27" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B14" s="27" t="n">
         <f aca="false">B13-C14</f>
@@ -10403,16 +10453,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="34" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B16" s="34" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E16" s="34" t="s">
         <v>29</v>
@@ -10427,7 +10477,7 @@
       </c>
       <c r="B17" s="35"/>
       <c r="D17" s="36" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E17" s="37"/>
     </row>
@@ -11151,7 +11201,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="4.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="45.57"/>
@@ -11770,7 +11820,7 @@
     </row>
     <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="20" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B34" s="21" t="n">
         <v>11</v>
@@ -11784,16 +11834,16 @@
       <c r="E34" s="17"/>
       <c r="F34" s="17"/>
       <c r="G34" s="22" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H34" s="23" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I34" s="23" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="J34" s="23" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="35" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11824,7 +11874,7 @@
     </row>
     <row r="36" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="20" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B36" s="21" t="n">
         <v>13</v>
@@ -11841,16 +11891,16 @@
         <v>76</v>
       </c>
       <c r="H36" s="23" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I36" s="23" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="J36" s="23"/>
     </row>
     <row r="37" s="24" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="20" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B37" s="21" t="n">
         <v>14</v>
@@ -11864,21 +11914,21 @@
       <c r="E37" s="17"/>
       <c r="F37" s="17"/>
       <c r="G37" s="22" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H37" s="23" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I37" s="23" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="J37" s="23" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" s="24" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="20" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B38" s="21" t="n">
         <v>15</v>
@@ -11892,16 +11942,16 @@
       <c r="E38" s="17"/>
       <c r="F38" s="17"/>
       <c r="G38" s="22" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H38" s="23" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="I38" s="23" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="J38" s="23" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11923,16 +11973,16 @@
         <v>76</v>
       </c>
       <c r="H39" s="19" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="I39" s="19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J39" s="19"/>
     </row>
     <row r="40" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B40" s="11" t="n">
         <v>17</v>
@@ -11949,16 +11999,16 @@
         <v>64</v>
       </c>
       <c r="H40" s="19" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="I40" s="19" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="J40" s="19"/>
     </row>
     <row r="41" s="26" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B41" s="11" t="n">
         <v>18</v>
@@ -11975,18 +12025,18 @@
         <v>36</v>
       </c>
       <c r="H41" s="19" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I41" s="19" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J41" s="19" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B42" s="11" t="n">
         <v>19</v>
@@ -12003,13 +12053,13 @@
         <v>36</v>
       </c>
       <c r="H42" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="I42" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="J42" s="19" t="s">
         <v>107</v>
-      </c>
-      <c r="I42" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="J42" s="19" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12042,7 +12092,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="20" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B44" s="21" t="n">
         <v>21</v>
@@ -12059,10 +12109,10 @@
         <v>36</v>
       </c>
       <c r="H44" s="23" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I44" s="23" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="J44" s="23"/>
     </row>
@@ -12084,7 +12134,7 @@
       <c r="E46" s="11"/>
       <c r="F46" s="11"/>
       <c r="G46" s="13" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H46" s="19"/>
       <c r="I46" s="19"/>
@@ -12093,13 +12143,13 @@
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="11"/>
       <c r="C47" s="16" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D47" s="11"/>
       <c r="E47" s="11"/>
       <c r="F47" s="11"/>
       <c r="G47" s="14" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H47" s="19"/>
       <c r="I47" s="19"/>
@@ -12107,7 +12157,7 @@
     </row>
     <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B48" s="11" t="n">
         <v>22</v>
@@ -12119,21 +12169,21 @@
       <c r="E48" s="17"/>
       <c r="F48" s="17"/>
       <c r="G48" s="14" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H48" s="19" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I48" s="19" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="J48" s="19" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B49" s="11" t="n">
         <v>23</v>
@@ -12148,16 +12198,16 @@
         <v>36</v>
       </c>
       <c r="H49" s="19" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="I49" s="19" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="J49" s="19"/>
     </row>
     <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B50" s="11" t="n">
         <v>24</v>
@@ -12172,16 +12222,16 @@
         <v>36</v>
       </c>
       <c r="H50" s="19" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I50" s="19" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="J50" s="19"/>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B51" s="11" t="n">
         <v>25</v>
@@ -12196,16 +12246,16 @@
         <v>36</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I51" s="19" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="J51" s="19"/>
     </row>
     <row r="52" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B52" s="11" t="n">
         <v>26</v>
@@ -12220,16 +12270,16 @@
         <v>76</v>
       </c>
       <c r="H52" s="19" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="I52" s="19" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J52" s="19"/>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B53" s="11" t="n">
         <v>27</v>
@@ -12244,16 +12294,16 @@
         <v>76</v>
       </c>
       <c r="H53" s="19" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="I53" s="19" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="J53" s="19"/>
     </row>
     <row r="54" s="24" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B54" s="11" t="n">
         <v>28</v>
@@ -12268,18 +12318,18 @@
         <v>36</v>
       </c>
       <c r="H54" s="19" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="I54" s="19" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="J54" s="19" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="55" s="24" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B55" s="11" t="n">
         <v>29</v>
@@ -12294,18 +12344,18 @@
         <v>76</v>
       </c>
       <c r="H55" s="19" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="I55" s="19" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="J55" s="19" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B56" s="11" t="n">
         <v>30</v>
@@ -12320,16 +12370,16 @@
         <v>36</v>
       </c>
       <c r="H56" s="19" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I56" s="19" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="J56" s="19"/>
     </row>
     <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B57" s="11" t="n">
         <v>31</v>
@@ -12344,16 +12394,16 @@
         <v>36</v>
       </c>
       <c r="H57" s="19" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I57" s="19" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="J57" s="19"/>
     </row>
     <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B58" s="11" t="n">
         <v>32</v>
@@ -12368,16 +12418,16 @@
         <v>36</v>
       </c>
       <c r="H58" s="19" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I58" s="19" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="J58" s="19"/>
     </row>
     <row r="59" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B59" s="11" t="n">
         <v>33</v>
@@ -12392,16 +12442,16 @@
         <v>36</v>
       </c>
       <c r="H59" s="19" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="I59" s="19" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="J59" s="19"/>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B60" s="11" t="n">
         <v>34</v>
@@ -12416,7 +12466,7 @@
         <v>64</v>
       </c>
       <c r="H60" s="19" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I60" s="19" t="s">
         <v>66</v>
@@ -12425,7 +12475,7 @@
     </row>
     <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B61" s="11" t="n">
         <v>35</v>
@@ -12440,10 +12490,10 @@
         <v>36</v>
       </c>
       <c r="H61" s="19" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="I61" s="19" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="J61" s="19"/>
     </row>

</xml_diff>